<commit_message>
Correct some incorrectly entered coefficients
</commit_message>
<xml_diff>
--- a/data-raw/0__Metabolic_Equations.xlsx
+++ b/data-raw/0__Metabolic_Equations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prhibbing\Desktop\PAutilities\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792583F2-D376-4E4B-A017-88E2DD976469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23818BB-5EDE-46A9-A9EA-CE5FF1D512A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{F5A1E7FC-EF51-4C1B-A3B3-D14B6D1B3683}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5A1E7FC-EF51-4C1B-A3B3-D14B6D1B3683}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>355.09550000000002</v>
+        <v>655.09550000000002</v>
       </c>
       <c r="E2">
         <v>9.5633999999999997</v>
@@ -560,7 +560,7 @@
         <v>1.8495999999999999</v>
       </c>
       <c r="H2">
-        <v>4.6756000000000002</v>
+        <v>-4.6756000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -583,7 +583,7 @@
         <v>5.0033000000000003</v>
       </c>
       <c r="H3">
-        <v>6.7549999999999999</v>
+        <v>-6.7549999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>